<commit_message>
new push at 3 pm
</commit_message>
<xml_diff>
--- a/FrameworkPOM/data/Chola.xlsx
+++ b/FrameworkPOM/data/Chola.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="TestDetails" sheetId="2" r:id="rId2"/>
     <sheet name="GridProperties" sheetId="3" r:id="rId3"/>
     <sheet name="MobileProperties" sheetId="4" r:id="rId4"/>
-    <sheet name="ObjectRepository" sheetId="5" r:id="rId5"/>
-    <sheet name="MobileRepository" sheetId="6" r:id="rId6"/>
+    <sheet name="WebObjectRepository" sheetId="5" r:id="rId5"/>
+    <sheet name="ObjectRepository" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -595,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -753,7 +753,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>